<commit_message>
include Tanix TX3 mini
</commit_message>
<xml_diff>
--- a/nbench/list2024.xlsx
+++ b/nbench/list2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\github\benchmark\nbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98204165-6695-42E8-AB9B-A315176CFF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35AD763-2E99-40ED-8879-49083E4D0B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="30" windowWidth="19515" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33270" yWindow="585" windowWidth="19515" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="184">
   <si>
     <t>CPU</t>
   </si>
@@ -575,6 +575,12 @@
   </si>
   <si>
     <t>Test Date</t>
+  </si>
+  <si>
+    <t>Tanix TX3 mini</t>
+  </si>
+  <si>
+    <t>Amlogic S905W</t>
   </si>
 </sst>
 </file>
@@ -699,6 +705,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,10 +720,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -996,11 +1002,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A198D7-6D1E-4BFD-BCE5-F3668492731D}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,10 +1083,10 @@
       <c r="I2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="13">
         <v>40892</v>
       </c>
-      <c r="L2" s="17"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1110,10 +1116,10 @@
       <c r="I3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="13">
         <v>41122</v>
       </c>
-      <c r="L3" s="17"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1143,10 +1149,10 @@
       <c r="I4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="13">
         <v>41487</v>
       </c>
-      <c r="L4" s="17"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1176,10 +1182,10 @@
       <c r="I5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="13">
         <v>41489</v>
       </c>
-      <c r="L5" s="17"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1209,10 +1215,10 @@
       <c r="I6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="13">
         <v>41122</v>
       </c>
-      <c r="L6" s="17"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1242,8 +1248,8 @@
       <c r="I7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="L7" s="17"/>
+      <c r="J7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1273,10 +1279,10 @@
       <c r="I8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="13">
         <v>41861</v>
       </c>
-      <c r="L8" s="17"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1306,10 +1312,10 @@
       <c r="I9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="13">
         <v>41861</v>
       </c>
-      <c r="L9" s="17"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1339,10 +1345,10 @@
       <c r="I10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="13">
         <v>41861</v>
       </c>
-      <c r="L10" s="17"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1372,10 +1378,10 @@
       <c r="I11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="13">
         <v>41861</v>
       </c>
-      <c r="L11" s="17"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1405,10 +1411,10 @@
       <c r="I12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="13">
         <v>42217</v>
       </c>
-      <c r="L12" s="17"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1438,10 +1444,10 @@
       <c r="I13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="13">
         <v>41797</v>
       </c>
-      <c r="L13" s="17"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1471,10 +1477,10 @@
       <c r="I14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="13">
         <v>40269</v>
       </c>
-      <c r="L14" s="17"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1504,10 +1510,10 @@
       <c r="I15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="13">
         <v>40017</v>
       </c>
-      <c r="L15" s="17"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1537,10 +1543,10 @@
       <c r="I16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="13">
         <v>40026</v>
       </c>
-      <c r="L16" s="17"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1570,10 +1576,10 @@
       <c r="I17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="13">
         <v>41496</v>
       </c>
-      <c r="L17" s="17"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1603,807 +1609,807 @@
       <c r="I18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="13">
         <v>42031</v>
       </c>
-      <c r="L18" s="17"/>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
       <c r="C19">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="D19" s="10">
-        <v>11.269</v>
+        <v>8.68</v>
       </c>
       <c r="E19" s="10">
-        <v>11.927</v>
+        <v>10.948</v>
       </c>
       <c r="F19" s="10">
-        <v>20.516999999999999</v>
+        <v>10.154999999999999</v>
       </c>
       <c r="G19" s="11">
-        <v>46.6</v>
+        <v>39.718000000000004</v>
       </c>
       <c r="H19" s="11">
-        <v>37</v>
+        <v>18.309999999999999</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="17">
-        <v>40672</v>
-      </c>
-      <c r="L19" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="J19" s="13">
+        <v>45319</v>
+      </c>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20">
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="D20" s="10">
-        <v>12.138</v>
+        <v>11.269</v>
       </c>
       <c r="E20" s="10">
-        <v>12.568</v>
+        <v>11.927</v>
       </c>
       <c r="F20" s="10">
-        <v>21.143999999999998</v>
+        <v>20.516999999999999</v>
       </c>
       <c r="G20" s="11">
-        <v>49.6</v>
+        <v>46.6</v>
       </c>
       <c r="H20" s="11">
-        <v>38.1</v>
+        <v>37</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="17">
-        <v>39919</v>
-      </c>
-      <c r="L20" s="17"/>
+        <v>37</v>
+      </c>
+      <c r="J20" s="13">
+        <v>40672</v>
+      </c>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C21">
-        <v>1860</v>
+        <v>2000</v>
       </c>
       <c r="D21" s="10">
-        <v>18.433</v>
+        <v>12.138</v>
       </c>
       <c r="E21" s="10">
-        <v>15.15</v>
+        <v>12.568</v>
       </c>
       <c r="F21" s="10">
-        <v>16.635999999999999</v>
+        <v>21.143999999999998</v>
       </c>
       <c r="G21" s="11">
-        <v>66</v>
+        <v>49.6</v>
       </c>
       <c r="H21" s="11">
-        <v>30</v>
+        <v>38.1</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" s="17">
-        <v>41788</v>
-      </c>
-      <c r="L21" s="17"/>
+        <v>39</v>
+      </c>
+      <c r="J21" s="13">
+        <v>39919</v>
+      </c>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>106</v>
       </c>
       <c r="C22">
-        <v>1800</v>
+        <v>1860</v>
       </c>
       <c r="D22" s="10">
-        <v>13.595000000000001</v>
+        <v>18.433</v>
       </c>
       <c r="E22" s="10">
-        <v>16.120999999999999</v>
+        <v>15.15</v>
       </c>
       <c r="F22" s="10">
-        <v>19.565999999999999</v>
+        <v>16.635999999999999</v>
       </c>
       <c r="G22" s="11">
-        <v>59.9</v>
+        <v>66</v>
       </c>
       <c r="H22" s="11">
-        <v>35.299999999999997</v>
+        <v>30</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J22" s="17">
-        <v>40672</v>
-      </c>
-      <c r="L22" s="17"/>
+        <v>45</v>
+      </c>
+      <c r="J22" s="13">
+        <v>41788</v>
+      </c>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="C23">
-        <v>1580</v>
+        <v>1800</v>
       </c>
       <c r="D23" s="10">
-        <v>19.981000000000002</v>
+        <v>13.595000000000001</v>
       </c>
       <c r="E23" s="10">
-        <v>16.207000000000001</v>
+        <v>16.120999999999999</v>
       </c>
       <c r="F23" s="10">
-        <v>18.001000000000001</v>
+        <v>19.565999999999999</v>
       </c>
       <c r="G23" s="11">
-        <v>71</v>
+        <v>59.9</v>
       </c>
       <c r="H23" s="11">
-        <v>32.5</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J23" s="17">
-        <v>41851</v>
-      </c>
-      <c r="L23" s="17"/>
+        <v>41</v>
+      </c>
+      <c r="J23" s="13">
+        <v>40672</v>
+      </c>
+      <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C24">
-        <v>1299</v>
+        <v>1580</v>
       </c>
       <c r="D24" s="10">
-        <v>19.050999999999998</v>
+        <v>19.981000000000002</v>
       </c>
       <c r="E24" s="10">
-        <v>17.286000000000001</v>
+        <v>16.207000000000001</v>
       </c>
       <c r="F24" s="10">
-        <v>25.289000000000001</v>
+        <v>18.001000000000001</v>
       </c>
       <c r="G24" s="11">
-        <v>72.2</v>
+        <v>71</v>
       </c>
       <c r="H24" s="11">
-        <v>45.6</v>
+        <v>32.5</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="17">
-        <v>41861</v>
-      </c>
-      <c r="L24" s="17"/>
+        <v>47</v>
+      </c>
+      <c r="J24" s="13">
+        <v>41851</v>
+      </c>
+      <c r="L24" s="13"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C25">
-        <v>2527</v>
+        <v>1299</v>
       </c>
       <c r="D25" s="10">
-        <v>28.488</v>
+        <v>19.050999999999998</v>
       </c>
       <c r="E25" s="10">
-        <v>17.780999999999999</v>
+        <v>17.286000000000001</v>
       </c>
       <c r="F25" s="10">
-        <v>36.673000000000002</v>
+        <v>25.289000000000001</v>
       </c>
       <c r="G25" s="11">
-        <v>87.2</v>
+        <v>72.2</v>
       </c>
       <c r="H25" s="11">
-        <v>66.099999999999994</v>
+        <v>45.6</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J25" s="17">
-        <v>41457</v>
-      </c>
-      <c r="L25" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="J25" s="13">
+        <v>41861</v>
+      </c>
+      <c r="L25" s="13"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C26">
-        <v>1600</v>
+        <v>2527</v>
       </c>
       <c r="D26" s="10">
-        <v>23.695</v>
+        <v>28.488</v>
       </c>
       <c r="E26" s="10">
-        <v>17.817</v>
+        <v>17.780999999999999</v>
       </c>
       <c r="F26" s="10">
-        <v>25.515999999999998</v>
+        <v>36.673000000000002</v>
       </c>
       <c r="G26" s="11">
-        <v>80.7</v>
+        <v>87.2</v>
       </c>
       <c r="H26" s="11">
-        <v>46</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J26" s="17">
-        <v>44089</v>
-      </c>
-      <c r="L26" s="17"/>
+        <v>58</v>
+      </c>
+      <c r="J26" s="13">
+        <v>41457</v>
+      </c>
+      <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C27">
-        <v>1400</v>
+        <v>1600</v>
       </c>
       <c r="D27" s="10">
-        <v>18.776</v>
+        <v>23.695</v>
       </c>
       <c r="E27" s="10">
-        <v>17.878</v>
+        <v>17.817</v>
       </c>
       <c r="F27" s="10">
-        <v>29.106000000000002</v>
+        <v>25.515999999999998</v>
       </c>
       <c r="G27" s="11">
-        <v>73.2</v>
+        <v>80.7</v>
       </c>
       <c r="H27" s="11">
-        <v>52.5</v>
+        <v>46</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J27" s="17">
-        <v>43641</v>
-      </c>
-      <c r="L27" s="17"/>
+      <c r="J27" s="13">
+        <v>44089</v>
+      </c>
+      <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C28">
-        <v>2607</v>
+        <v>1400</v>
       </c>
       <c r="D28" s="10">
-        <v>18.265000000000001</v>
+        <v>18.776</v>
       </c>
       <c r="E28" s="10">
-        <v>18.957999999999998</v>
+        <v>17.878</v>
       </c>
       <c r="F28" s="10">
-        <v>31.843</v>
+        <v>29.106000000000002</v>
       </c>
       <c r="G28" s="11">
-        <v>74.8</v>
+        <v>73.2</v>
       </c>
       <c r="H28" s="11">
-        <v>57.4</v>
+        <v>52.5</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J28" s="17">
-        <v>41151</v>
-      </c>
-      <c r="L28" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="J28" s="13">
+        <v>43641</v>
+      </c>
+      <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C29">
-        <v>2100</v>
+        <v>2607</v>
       </c>
       <c r="D29" s="10">
-        <v>14.395</v>
+        <v>18.265000000000001</v>
       </c>
       <c r="E29" s="10">
-        <v>19.298999999999999</v>
+        <v>18.957999999999998</v>
       </c>
       <c r="F29" s="10">
-        <v>23.132000000000001</v>
+        <v>31.843</v>
       </c>
       <c r="G29" s="11">
-        <v>68.2</v>
+        <v>74.8</v>
       </c>
       <c r="H29" s="11">
-        <v>41.7</v>
+        <v>57.4</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J29" s="17">
-        <v>40060</v>
-      </c>
-      <c r="L29" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="J29" s="13">
+        <v>41151</v>
+      </c>
+      <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C30">
-        <v>2266</v>
+        <v>2100</v>
       </c>
       <c r="D30" s="10">
-        <v>28.631</v>
+        <v>14.395</v>
       </c>
       <c r="E30" s="10">
-        <v>19.780999999999999</v>
+        <v>19.298999999999999</v>
       </c>
       <c r="F30" s="10">
-        <v>31.140999999999998</v>
+        <v>23.132000000000001</v>
       </c>
       <c r="G30" s="11">
-        <v>92.9</v>
+        <v>68.2</v>
       </c>
       <c r="H30" s="11">
-        <v>56.1</v>
+        <v>41.7</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J30" s="17">
-        <v>42713</v>
-      </c>
-      <c r="L30" s="17"/>
+        <v>43</v>
+      </c>
+      <c r="J30" s="13">
+        <v>40060</v>
+      </c>
+      <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="C31">
-        <v>2043</v>
+        <v>2266</v>
       </c>
       <c r="D31" s="10">
-        <v>19.359000000000002</v>
+        <v>28.631</v>
       </c>
       <c r="E31" s="10">
-        <v>19.808</v>
+        <v>19.780999999999999</v>
       </c>
       <c r="F31" s="10">
-        <v>33.182000000000002</v>
+        <v>31.140999999999998</v>
       </c>
       <c r="G31" s="11">
-        <v>78.599999999999994</v>
+        <v>92.9</v>
       </c>
       <c r="H31" s="11">
-        <v>59.8</v>
+        <v>56.1</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J31" s="17">
-        <v>41919</v>
-      </c>
-      <c r="L31" s="17"/>
+        <v>60</v>
+      </c>
+      <c r="J31" s="13">
+        <v>42713</v>
+      </c>
+      <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C32">
-        <v>2832</v>
+        <v>2043</v>
       </c>
       <c r="D32" s="10">
-        <v>33.670999999999999</v>
+        <v>19.359000000000002</v>
       </c>
       <c r="E32" s="10">
-        <v>23.584</v>
+        <v>19.808</v>
       </c>
       <c r="F32" s="10">
-        <v>36.384</v>
+        <v>33.182000000000002</v>
       </c>
       <c r="G32" s="11">
-        <v>110.1</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="H32" s="11">
-        <v>65.599999999999994</v>
+        <v>59.8</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J32" s="17">
-        <v>42443</v>
-      </c>
-      <c r="L32" s="17"/>
+        <v>52</v>
+      </c>
+      <c r="J32" s="13">
+        <v>41919</v>
+      </c>
+      <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>133</v>
       </c>
       <c r="C33">
-        <v>3066</v>
+        <v>2832</v>
       </c>
       <c r="D33" s="10">
-        <v>28.776</v>
+        <v>33.670999999999999</v>
       </c>
       <c r="E33" s="10">
-        <v>23.881</v>
+        <v>23.584</v>
       </c>
       <c r="F33" s="10">
-        <v>47.396000000000001</v>
+        <v>36.384</v>
       </c>
       <c r="G33" s="11">
-        <v>103.658</v>
+        <v>110.1</v>
       </c>
       <c r="H33" s="11">
-        <v>85.453000000000003</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="J33" s="17">
-        <v>44691</v>
-      </c>
-      <c r="K33" s="5"/>
-      <c r="L33" s="17"/>
+        <v>62</v>
+      </c>
+      <c r="J33" s="13">
+        <v>42443</v>
+      </c>
+      <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>175</v>
       </c>
       <c r="C34">
-        <v>3200</v>
+        <v>3066</v>
       </c>
       <c r="D34" s="10">
-        <v>37.845999999999997</v>
+        <v>28.776</v>
       </c>
       <c r="E34" s="10">
-        <v>23.882000000000001</v>
+        <v>23.881</v>
       </c>
       <c r="F34" s="10">
-        <v>47.436999999999998</v>
+        <v>47.396000000000001</v>
       </c>
       <c r="G34" s="11">
-        <v>116.6</v>
+        <v>103.658</v>
       </c>
       <c r="H34" s="11">
-        <v>85.5</v>
+        <v>85.453000000000003</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J34" s="17">
-        <v>41537</v>
-      </c>
-      <c r="L34" s="17"/>
+        <v>176</v>
+      </c>
+      <c r="J34" s="13">
+        <v>44691</v>
+      </c>
+      <c r="K34" s="5"/>
+      <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C35">
-        <v>2667</v>
+        <v>3200</v>
       </c>
       <c r="D35" s="10">
-        <v>24.206</v>
+        <v>37.845999999999997</v>
       </c>
       <c r="E35" s="10">
-        <v>24.602</v>
+        <v>23.882000000000001</v>
       </c>
       <c r="F35" s="10">
-        <v>41.085000000000001</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>10</v>
+        <v>47.436999999999998</v>
+      </c>
+      <c r="G35" s="11">
+        <v>116.6</v>
+      </c>
+      <c r="H35" s="11">
+        <v>85.5</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J35" s="17">
-        <v>40683</v>
-      </c>
-      <c r="L35" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="J35" s="13">
+        <v>41537</v>
+      </c>
+      <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C36">
-        <v>2829</v>
+        <v>2667</v>
       </c>
       <c r="D36" s="10">
-        <v>21.475999999999999</v>
+        <v>24.206</v>
       </c>
       <c r="E36" s="10">
-        <v>25.608000000000001</v>
+        <v>24.602</v>
       </c>
       <c r="F36" s="10">
-        <v>30.663</v>
-      </c>
-      <c r="G36" s="11">
-        <v>95.2</v>
-      </c>
-      <c r="H36" s="11">
-        <v>55.3</v>
+        <v>41.085000000000001</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J36" s="17">
-        <v>39896</v>
-      </c>
-      <c r="L36" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="J36" s="13">
+        <v>40683</v>
+      </c>
+      <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C37">
-        <v>3352</v>
+        <v>2829</v>
       </c>
       <c r="D37" s="10">
-        <v>28.021999999999998</v>
+        <v>21.475999999999999</v>
       </c>
       <c r="E37" s="10">
-        <v>32.585999999999999</v>
+        <v>25.608000000000001</v>
       </c>
       <c r="F37" s="10">
-        <v>44.103999999999999</v>
+        <v>30.663</v>
       </c>
       <c r="G37" s="11">
-        <v>122.4</v>
+        <v>95.2</v>
       </c>
       <c r="H37" s="11">
-        <v>79.2</v>
+        <v>55.3</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J37" s="17">
-        <v>42315</v>
-      </c>
-      <c r="L37" s="17"/>
+        <v>56</v>
+      </c>
+      <c r="J37" s="13">
+        <v>39896</v>
+      </c>
+      <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>138</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38">
         <v>3352</v>
       </c>
       <c r="D38" s="10">
-        <v>25.033999999999999</v>
+        <v>28.021999999999998</v>
       </c>
       <c r="E38" s="10">
-        <v>32.850999999999999</v>
+        <v>32.585999999999999</v>
       </c>
       <c r="F38" s="10">
-        <v>40.966999999999999</v>
+        <v>44.103999999999999</v>
       </c>
       <c r="G38" s="11">
-        <v>117.2</v>
+        <v>122.4</v>
       </c>
       <c r="H38" s="11">
-        <v>73.900000000000006</v>
+        <v>79.2</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J38" s="17">
+      <c r="J38" s="13">
         <v>42315</v>
       </c>
-      <c r="L38" s="17"/>
+      <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="C39">
-        <v>2300</v>
+        <v>3352</v>
       </c>
       <c r="D39" s="10">
-        <v>39.049999999999997</v>
+        <v>25.033999999999999</v>
       </c>
       <c r="E39" s="10">
-        <v>33.215000000000003</v>
+        <v>32.850999999999999</v>
       </c>
       <c r="F39" s="10">
-        <v>54.26</v>
+        <v>40.966999999999999</v>
       </c>
       <c r="G39" s="11">
-        <v>142.69999999999999</v>
+        <v>117.2</v>
       </c>
       <c r="H39" s="11">
-        <v>97.8</v>
+        <v>73.900000000000006</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J39" s="17">
-        <v>42397</v>
-      </c>
-      <c r="L39" s="17"/>
+        <v>67</v>
+      </c>
+      <c r="J39" s="13">
+        <v>42315</v>
+      </c>
+      <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="B40" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="C40">
-        <v>2500</v>
+        <v>2300</v>
       </c>
       <c r="D40" s="10">
-        <v>40.698999999999998</v>
+        <v>39.049999999999997</v>
       </c>
       <c r="E40" s="10">
-        <v>37.018000000000001</v>
+        <v>33.215000000000003</v>
       </c>
       <c r="F40" s="10">
-        <v>52.634999999999998</v>
+        <v>54.26</v>
       </c>
       <c r="G40" s="11">
-        <v>154.5</v>
+        <v>142.69999999999999</v>
       </c>
       <c r="H40" s="11">
-        <v>94.9</v>
+        <v>97.8</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J40" s="17">
+        <v>10</v>
+      </c>
+      <c r="J40" s="13">
         <v>42397</v>
       </c>
-      <c r="L40" s="17"/>
+      <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C41">
-        <v>2600</v>
+        <v>2500</v>
       </c>
       <c r="D41" s="10">
-        <v>45.381999999999998</v>
+        <v>40.698999999999998</v>
       </c>
       <c r="E41" s="10">
-        <v>40.313000000000002</v>
+        <v>37.018000000000001</v>
       </c>
       <c r="F41" s="10">
-        <v>61.804000000000002</v>
+        <v>52.634999999999998</v>
       </c>
       <c r="G41" s="11">
-        <v>169.9</v>
+        <v>154.5</v>
       </c>
       <c r="H41" s="11">
-        <v>111.4</v>
+        <v>94.9</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J41" s="17">
-        <v>42817</v>
-      </c>
-      <c r="L41" s="17"/>
+        <v>71</v>
+      </c>
+      <c r="J41" s="13">
+        <v>42397</v>
+      </c>
+      <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="C42">
-        <v>2700</v>
+        <v>2600</v>
       </c>
       <c r="D42" s="10">
-        <v>54.363</v>
+        <v>45.381999999999998</v>
       </c>
       <c r="E42" s="10">
-        <v>41.972000000000001</v>
+        <v>40.313000000000002</v>
       </c>
       <c r="F42" s="10">
-        <v>106.893</v>
+        <v>61.804000000000002</v>
       </c>
       <c r="G42" s="11">
-        <v>187.91900000000001</v>
+        <v>169.9</v>
       </c>
       <c r="H42" s="11">
-        <v>192.7</v>
+        <v>111.4</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="J42" s="17">
-        <v>44153</v>
-      </c>
-      <c r="L42" s="17"/>
+        <v>73</v>
+      </c>
+      <c r="J42" s="13">
+        <v>42817</v>
+      </c>
+      <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B43" t="s">
         <v>166</v>
@@ -2412,206 +2418,239 @@
         <v>2700</v>
       </c>
       <c r="D43" s="10">
-        <v>57.2</v>
+        <v>54.363</v>
       </c>
       <c r="E43" s="10">
-        <v>43.731999999999999</v>
+        <v>41.972000000000001</v>
       </c>
       <c r="F43" s="10">
-        <v>107.95399999999999</v>
+        <v>106.893</v>
       </c>
       <c r="G43" s="11">
-        <v>196.6</v>
+        <v>187.91900000000001</v>
       </c>
       <c r="H43" s="11">
-        <v>194.6</v>
-      </c>
-      <c r="J43" s="17">
-        <v>44155</v>
-      </c>
-      <c r="L43" s="17"/>
+        <v>192.7</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J43" s="13">
+        <v>44153</v>
+      </c>
+      <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="B44" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C44">
-        <v>2600</v>
+        <v>2700</v>
       </c>
       <c r="D44" s="10">
-        <v>55.045999999999999</v>
+        <v>57.2</v>
       </c>
       <c r="E44" s="10">
-        <v>44.618000000000002</v>
+        <v>43.731999999999999</v>
       </c>
       <c r="F44" s="10">
-        <v>73.569999999999993</v>
+        <v>107.95399999999999</v>
       </c>
       <c r="G44" s="11">
-        <v>195.6</v>
+        <v>196.6</v>
       </c>
       <c r="H44" s="11">
-        <v>132.6</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="J44" s="17">
-        <v>43355</v>
-      </c>
-      <c r="K44" s="7"/>
-      <c r="L44" s="17"/>
+        <v>194.6</v>
+      </c>
+      <c r="J44" s="13">
+        <v>44155</v>
+      </c>
+      <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="C45">
         <v>2600</v>
       </c>
       <c r="D45" s="10">
-        <v>63.682000000000002</v>
+        <v>55.045999999999999</v>
       </c>
       <c r="E45" s="10">
-        <v>45.731999999999999</v>
+        <v>44.618000000000002</v>
       </c>
       <c r="F45" s="10">
-        <v>68.159000000000006</v>
+        <v>73.569999999999993</v>
       </c>
       <c r="G45" s="11">
-        <v>211.2</v>
+        <v>195.6</v>
       </c>
       <c r="H45" s="11">
-        <v>122.9</v>
+        <v>132.6</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J45" s="17">
-        <v>43146</v>
+        <v>77</v>
+      </c>
+      <c r="J45" s="13">
+        <v>43355</v>
       </c>
       <c r="K45" s="7"/>
-      <c r="L45" s="17"/>
+      <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46">
-        <v>2500</v>
+        <v>2600</v>
       </c>
       <c r="D46" s="10">
-        <v>50.423000000000002</v>
+        <v>63.682000000000002</v>
       </c>
       <c r="E46" s="10">
-        <v>46.116999999999997</v>
+        <v>45.731999999999999</v>
       </c>
       <c r="F46" s="10">
-        <v>70.039000000000001</v>
+        <v>68.159000000000006</v>
       </c>
       <c r="G46" s="11">
-        <v>192</v>
+        <v>211.2</v>
       </c>
       <c r="H46" s="11">
-        <v>126.3</v>
+        <v>122.9</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J46" s="17">
+      <c r="J46" s="13">
         <v>43146</v>
       </c>
-      <c r="K46" s="5"/>
-      <c r="L46" s="17"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="C47">
-        <v>3600</v>
+        <v>2500</v>
       </c>
       <c r="D47" s="10">
-        <v>77.174000000000007</v>
+        <v>50.423000000000002</v>
       </c>
       <c r="E47" s="10">
-        <v>56.761000000000003</v>
+        <v>46.116999999999997</v>
       </c>
       <c r="F47" s="10">
-        <v>138.00299999999999</v>
+        <v>70.039000000000001</v>
       </c>
       <c r="G47" s="11">
-        <v>259.47000000000003</v>
+        <v>192</v>
       </c>
       <c r="H47" s="11">
-        <v>248.81200000000001</v>
+        <v>126.3</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="J47" s="18">
-        <v>45211</v>
+        <v>10</v>
+      </c>
+      <c r="J47" s="13">
+        <v>43146</v>
       </c>
       <c r="K47" s="5"/>
-      <c r="L47" s="17"/>
+      <c r="L47" s="13"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48">
+        <v>3600</v>
+      </c>
+      <c r="D48" s="10">
+        <v>77.174000000000007</v>
+      </c>
+      <c r="E48" s="10">
+        <v>56.761000000000003</v>
+      </c>
+      <c r="F48" s="10">
+        <v>138.00299999999999</v>
+      </c>
+      <c r="G48" s="11">
+        <v>259.47000000000003</v>
+      </c>
+      <c r="H48" s="11">
+        <v>248.81200000000001</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="J48" s="14">
+        <v>45211</v>
+      </c>
+      <c r="K48" s="5"/>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>167</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>168</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>2667</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J48" s="17">
-        <v>43956</v>
-      </c>
-      <c r="L48" s="17"/>
-    </row>
-    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
-      <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J49" s="13">
+        <v>43956</v>
+      </c>
+      <c r="L49" s="13"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F50" s="10"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
       <c r="J50" s="7"/>
     </row>
-    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F51" s="10"/>
       <c r="J51" s="7"/>
     </row>
-    <row r="52" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J52" s="7"/>
     </row>
-    <row r="53" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J53" s="7"/>
     </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J54" s="7"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J48">
-    <sortCondition ref="E2:E48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J49">
+    <sortCondition ref="E2:E49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7242,7 +7281,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -7254,10 +7293,10 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -7265,7 +7304,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
+      <c r="A2" s="15"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -7275,8 +7314,8 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
@@ -7423,22 +7462,22 @@
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="17">
         <v>2.7480000000000002</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="17">
         <v>3.282</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="17">
         <v>3.7109999999999999</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="18">
         <v>12.8</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="18">
         <v>6.69</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7446,33 +7485,33 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="17">
         <v>3.665</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="17">
         <v>5.46</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="17">
         <v>4.6849999999999996</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="18">
         <v>18.399999999999999</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="18">
         <v>8.4499999999999993</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7480,12 +7519,12 @@
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -7629,22 +7668,22 @@
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="17">
         <v>4.5910000000000002</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="17">
         <v>9.8949999999999996</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="17">
         <v>9.0860000000000003</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="18">
         <v>28.5</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="18">
         <v>16.399999999999999</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7652,12 +7691,12 @@
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="15"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -8281,7 +8320,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -8293,10 +8332,10 @@
       <c r="D48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G48" s="1" t="s">
@@ -8304,7 +8343,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="1" t="s">
         <v>2</v>
       </c>
@@ -8314,14 +8353,30 @@
       <c r="D49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
       <c r="G49" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="F48:F49"/>
@@ -8330,22 +8385,6 @@
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="http://pdadb.net/index.php?m=cpu&amp;id=a6422&amp;c=samsung_s5p6422" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>

<commit_message>
include M1 and 13700T
</commit_message>
<xml_diff>
--- a/nbench/list2024.xlsx
+++ b/nbench/list2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\github\benchmark\nbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35AD763-2E99-40ED-8879-49083E4D0B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7D4B20-EEAC-49BA-956B-203E16CA8705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33270" yWindow="585" windowWidth="19515" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16995" yWindow="1995" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="221">
   <si>
     <t>CPU</t>
   </si>
@@ -581,6 +581,117 @@
   </si>
   <si>
     <t>Amlogic S905W</t>
+  </si>
+  <si>
+    <t>HP mini 400 G9</t>
+  </si>
+  <si>
+    <t>i7 13700T</t>
+  </si>
+  <si>
+    <t>Mark PC</t>
+  </si>
+  <si>
+    <t>49.100s</t>
+  </si>
+  <si>
+    <t>33.800s</t>
+  </si>
+  <si>
+    <t>42.056s</t>
+  </si>
+  <si>
+    <t>49.400s</t>
+  </si>
+  <si>
+    <t>43.033s</t>
+  </si>
+  <si>
+    <t>17.437s</t>
+  </si>
+  <si>
+    <t>30.700s</t>
+  </si>
+  <si>
+    <t>06.917s</t>
+  </si>
+  <si>
+    <t>08.748s</t>
+  </si>
+  <si>
+    <t>10.164s</t>
+  </si>
+  <si>
+    <t>10.712s</t>
+  </si>
+  <si>
+    <t>12.264s</t>
+  </si>
+  <si>
+    <t>13.145s</t>
+  </si>
+  <si>
+    <t>16.300s</t>
+  </si>
+  <si>
+    <t>34.300s</t>
+  </si>
+  <si>
+    <t>14.700s</t>
+  </si>
+  <si>
+    <t>18.923s</t>
+  </si>
+  <si>
+    <t>18.473s</t>
+  </si>
+  <si>
+    <t>25.700s</t>
+  </si>
+  <si>
+    <t>22.112s</t>
+  </si>
+  <si>
+    <t>10.044s</t>
+  </si>
+  <si>
+    <t>Proxmox 1226</t>
+  </si>
+  <si>
+    <t>E3-1226 v3</t>
+  </si>
+  <si>
+    <t>50.264s</t>
+  </si>
+  <si>
+    <t>14.800s</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4</t>
+  </si>
+  <si>
+    <t>BCM2711</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3</t>
+  </si>
+  <si>
+    <t>BCM2837 B0</t>
+  </si>
+  <si>
+    <t>HP mini 800 G4</t>
+  </si>
+  <si>
+    <t>i5 8500T</t>
+  </si>
+  <si>
+    <t>10.900s</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MacBook Air 2020 </t>
   </si>
 </sst>
 </file>
@@ -624,7 +735,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -661,6 +772,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -675,7 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -720,6 +849,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1002,11 +1139,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A198D7-6D1E-4BFD-BCE5-F3668492731D}">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,10 +1193,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C2">
@@ -1122,10 +1259,10 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="19" t="s">
         <v>146</v>
       </c>
       <c r="C4">
@@ -1188,10 +1325,10 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="19" t="s">
         <v>147</v>
       </c>
       <c r="C6">
@@ -1252,10 +1389,10 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="19" t="s">
         <v>143</v>
       </c>
       <c r="C8">
@@ -1285,13 +1422,13 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="20">
         <v>933</v>
       </c>
       <c r="D9" s="10">
@@ -1318,10 +1455,10 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="19" t="s">
         <v>144</v>
       </c>
       <c r="C10">
@@ -1384,10 +1521,10 @@
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="19" t="s">
         <v>116</v>
       </c>
       <c r="C12">
@@ -1417,13 +1554,13 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="20">
         <v>1200</v>
       </c>
       <c r="D13" s="10">
@@ -1450,13 +1587,13 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="20">
         <v>1666</v>
       </c>
       <c r="D14" s="10">
@@ -1516,13 +1653,13 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="20">
         <v>1600</v>
       </c>
       <c r="D16" s="10">
@@ -1549,13 +1686,13 @@
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="20">
         <v>1666</v>
       </c>
       <c r="D17" s="10">
@@ -1583,1074 +1720,1225 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18">
+        <v>1200</v>
+      </c>
+      <c r="D18" s="10">
+        <v>6.78</v>
+      </c>
+      <c r="E18" s="10">
+        <v>9.5239999999999991</v>
+      </c>
+      <c r="F18" s="10">
+        <v>9.1739999999999995</v>
+      </c>
+      <c r="G18" s="11">
+        <v>33</v>
+      </c>
+      <c r="H18" s="11">
+        <v>16.5</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="13">
+        <v>45298</v>
+      </c>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>1512</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D19" s="10">
         <v>4.5910000000000002</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E19" s="10">
         <v>9.8949999999999996</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F19" s="10">
         <v>9.0860000000000003</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G19" s="11">
         <v>28.5</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H19" s="11">
         <v>16.399999999999999</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="13">
+      <c r="I19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="13">
         <v>42031</v>
-      </c>
-      <c r="L18" s="13"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>182</v>
-      </c>
-      <c r="B19" t="s">
-        <v>183</v>
-      </c>
-      <c r="C19">
-        <v>1200</v>
-      </c>
-      <c r="D19" s="10">
-        <v>8.68</v>
-      </c>
-      <c r="E19" s="10">
-        <v>10.948</v>
-      </c>
-      <c r="F19" s="10">
-        <v>10.154999999999999</v>
-      </c>
-      <c r="G19" s="11">
-        <v>39.718000000000004</v>
-      </c>
-      <c r="H19" s="11">
-        <v>18.309999999999999</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="13">
-        <v>45319</v>
       </c>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
       <c r="C20">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="D20" s="10">
-        <v>11.269</v>
+        <v>8.68</v>
       </c>
       <c r="E20" s="10">
-        <v>11.927</v>
+        <v>10.948</v>
       </c>
       <c r="F20" s="10">
-        <v>20.516999999999999</v>
+        <v>10.154999999999999</v>
       </c>
       <c r="G20" s="11">
-        <v>46.6</v>
+        <v>39.718000000000004</v>
       </c>
       <c r="H20" s="11">
-        <v>37</v>
+        <v>18.309999999999999</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="J20" s="13">
-        <v>40672</v>
+        <v>45319</v>
       </c>
       <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21">
+        <v>1800</v>
+      </c>
+      <c r="D21" s="10">
+        <v>11.269</v>
+      </c>
+      <c r="E21" s="10">
+        <v>11.927</v>
+      </c>
+      <c r="F21" s="10">
+        <v>20.516999999999999</v>
+      </c>
+      <c r="G21" s="11">
+        <v>46.6</v>
+      </c>
+      <c r="H21" s="11">
+        <v>37</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="J21" s="13">
+        <v>40672</v>
+      </c>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C21">
+      <c r="C22" s="20">
         <v>2000</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D22" s="10">
         <v>12.138</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E22" s="10">
         <v>12.568</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F22" s="10">
         <v>21.143999999999998</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G22" s="11">
         <v>49.6</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H22" s="11">
         <v>38.1</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="13">
+      <c r="I22" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="J22" s="13">
         <v>39919</v>
       </c>
-      <c r="L21" s="13"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C22">
+      <c r="C23" s="20">
         <v>1860</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D23" s="10">
         <v>18.433</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="10">
         <v>15.15</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F23" s="10">
         <v>16.635999999999999</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G23" s="11">
         <v>66</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H23" s="11">
         <v>30</v>
       </c>
-      <c r="I22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J22" s="13">
+      <c r="I23" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="J23" s="13">
         <v>41788</v>
-      </c>
-      <c r="L22" s="13"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23">
-        <v>1800</v>
-      </c>
-      <c r="D23" s="10">
-        <v>13.595000000000001</v>
-      </c>
-      <c r="E23" s="10">
-        <v>16.120999999999999</v>
-      </c>
-      <c r="F23" s="10">
-        <v>19.565999999999999</v>
-      </c>
-      <c r="G23" s="11">
-        <v>59.9</v>
-      </c>
-      <c r="H23" s="11">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="13">
-        <v>40672</v>
       </c>
       <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24">
+        <v>1800</v>
+      </c>
+      <c r="D24" s="10">
+        <v>13.595000000000001</v>
+      </c>
+      <c r="E24" s="10">
+        <v>16.120999999999999</v>
+      </c>
+      <c r="F24" s="10">
+        <v>19.565999999999999</v>
+      </c>
+      <c r="G24" s="11">
+        <v>59.9</v>
+      </c>
+      <c r="H24" s="11">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J24" s="13">
+        <v>40672</v>
+      </c>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C24">
+      <c r="C25" s="20">
         <v>1580</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D25" s="10">
         <v>19.981000000000002</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E25" s="10">
         <v>16.207000000000001</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F25" s="10">
         <v>18.001000000000001</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G25" s="11">
         <v>71</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H25" s="11">
         <v>32.5</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J24" s="13">
+      <c r="I25" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="J25" s="13">
         <v>41851</v>
       </c>
-      <c r="L24" s="13"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="L25" s="13"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C25">
+      <c r="C26" s="20">
         <v>1299</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D26" s="10">
         <v>19.050999999999998</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E26" s="10">
         <v>17.286000000000001</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F26" s="10">
         <v>25.289000000000001</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G26" s="11">
         <v>72.2</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H26" s="11">
         <v>45.6</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J25" s="13">
+      <c r="I26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="13">
         <v>41861</v>
-      </c>
-      <c r="L25" s="13"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>137</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26">
-        <v>2527</v>
-      </c>
-      <c r="D26" s="10">
-        <v>28.488</v>
-      </c>
-      <c r="E26" s="10">
-        <v>17.780999999999999</v>
-      </c>
-      <c r="F26" s="10">
-        <v>36.673000000000002</v>
-      </c>
-      <c r="G26" s="11">
-        <v>87.2</v>
-      </c>
-      <c r="H26" s="11">
-        <v>66.099999999999994</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J26" s="13">
-        <v>41457</v>
       </c>
       <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27">
+        <v>2527</v>
+      </c>
+      <c r="D27" s="10">
+        <v>28.488</v>
+      </c>
+      <c r="E27" s="10">
+        <v>17.780999999999999</v>
+      </c>
+      <c r="F27" s="10">
+        <v>36.673000000000002</v>
+      </c>
+      <c r="G27" s="11">
+        <v>87.2</v>
+      </c>
+      <c r="H27" s="11">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="J27" s="13">
+        <v>41457</v>
+      </c>
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>1600</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D28" s="10">
         <v>23.695</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E28" s="10">
         <v>17.817</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F28" s="10">
         <v>25.515999999999998</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G28" s="11">
         <v>80.7</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H28" s="11">
         <v>46</v>
       </c>
-      <c r="I27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J27" s="13">
+      <c r="I28" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="J28" s="13">
         <v>44089</v>
       </c>
-      <c r="L27" s="13"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="C28">
+      <c r="C29" s="20">
         <v>1400</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D29" s="10">
         <v>18.776</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E29" s="10">
         <v>17.878</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F29" s="10">
         <v>29.106000000000002</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G29" s="11">
         <v>73.2</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H29" s="11">
         <v>52.5</v>
       </c>
-      <c r="I28" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J28" s="13">
+      <c r="I29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="13">
         <v>43641</v>
-      </c>
-      <c r="L28" s="13"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29">
-        <v>2607</v>
-      </c>
-      <c r="D29" s="10">
-        <v>18.265000000000001</v>
-      </c>
-      <c r="E29" s="10">
-        <v>18.957999999999998</v>
-      </c>
-      <c r="F29" s="10">
-        <v>31.843</v>
-      </c>
-      <c r="G29" s="11">
-        <v>74.8</v>
-      </c>
-      <c r="H29" s="11">
-        <v>57.4</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="13">
-        <v>41151</v>
       </c>
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>213</v>
       </c>
       <c r="C30">
-        <v>2100</v>
+        <v>1500</v>
       </c>
       <c r="D30" s="10">
-        <v>14.395</v>
+        <v>15.319000000000001</v>
       </c>
       <c r="E30" s="10">
-        <v>19.298999999999999</v>
+        <v>18.061</v>
       </c>
       <c r="F30" s="10">
-        <v>23.132000000000001</v>
+        <v>34.619999999999997</v>
       </c>
       <c r="G30" s="11">
-        <v>68.2</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="H30" s="11">
-        <v>41.7</v>
+        <v>62.4</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="J30" s="13">
-        <v>40060</v>
+        <v>45561</v>
       </c>
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="B31" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="C31">
-        <v>2266</v>
+        <v>2607</v>
       </c>
       <c r="D31" s="10">
-        <v>28.631</v>
+        <v>18.265000000000001</v>
       </c>
       <c r="E31" s="10">
-        <v>19.780999999999999</v>
+        <v>18.957999999999998</v>
       </c>
       <c r="F31" s="10">
-        <v>31.140999999999998</v>
+        <v>31.843</v>
       </c>
       <c r="G31" s="11">
-        <v>92.9</v>
+        <v>74.8</v>
       </c>
       <c r="H31" s="11">
-        <v>56.1</v>
+        <v>57.4</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>60</v>
+        <v>193</v>
       </c>
       <c r="J31" s="13">
-        <v>42713</v>
+        <v>41151</v>
       </c>
       <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32">
+        <v>2100</v>
+      </c>
+      <c r="D32" s="10">
+        <v>14.395</v>
+      </c>
+      <c r="E32" s="10">
+        <v>19.298999999999999</v>
+      </c>
+      <c r="F32" s="10">
+        <v>23.132000000000001</v>
+      </c>
+      <c r="G32" s="11">
+        <v>68.2</v>
+      </c>
+      <c r="H32" s="11">
+        <v>41.7</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" s="13">
+        <v>40060</v>
+      </c>
+      <c r="L32" s="13"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="20">
+        <v>2266</v>
+      </c>
+      <c r="D33" s="10">
+        <v>28.631</v>
+      </c>
+      <c r="E33" s="10">
+        <v>19.780999999999999</v>
+      </c>
+      <c r="F33" s="10">
+        <v>31.140999999999998</v>
+      </c>
+      <c r="G33" s="11">
+        <v>92.9</v>
+      </c>
+      <c r="H33" s="11">
+        <v>56.1</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J33" s="13">
+        <v>42713</v>
+      </c>
+      <c r="L33" s="13"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C32">
+      <c r="C34" s="20">
         <v>2043</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D34" s="10">
         <v>19.359000000000002</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E34" s="10">
         <v>19.808</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F34" s="10">
         <v>33.182000000000002</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G34" s="11">
         <v>78.599999999999994</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H34" s="11">
         <v>59.8</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J32" s="13">
+      <c r="I34" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="J34" s="13">
         <v>41919</v>
       </c>
-      <c r="L32" s="13"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" t="s">
-        <v>133</v>
-      </c>
-      <c r="C33">
-        <v>2832</v>
-      </c>
-      <c r="D33" s="10">
-        <v>33.670999999999999</v>
-      </c>
-      <c r="E33" s="10">
-        <v>23.584</v>
-      </c>
-      <c r="F33" s="10">
-        <v>36.384</v>
-      </c>
-      <c r="G33" s="11">
-        <v>110.1</v>
-      </c>
-      <c r="H33" s="11">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J33" s="13">
-        <v>42443</v>
-      </c>
-      <c r="L33" s="13"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>174</v>
-      </c>
-      <c r="B34" t="s">
-        <v>175</v>
-      </c>
-      <c r="C34">
-        <v>3066</v>
-      </c>
-      <c r="D34" s="10">
-        <v>28.776</v>
-      </c>
-      <c r="E34" s="10">
-        <v>23.881</v>
-      </c>
-      <c r="F34" s="10">
-        <v>47.396000000000001</v>
-      </c>
-      <c r="G34" s="11">
-        <v>103.658</v>
-      </c>
-      <c r="H34" s="11">
-        <v>85.453000000000003</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="J34" s="13">
-        <v>44691</v>
-      </c>
-      <c r="K34" s="5"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C35">
-        <v>3200</v>
+        <v>2832</v>
       </c>
       <c r="D35" s="10">
-        <v>37.845999999999997</v>
+        <v>33.670999999999999</v>
       </c>
       <c r="E35" s="10">
-        <v>23.882000000000001</v>
+        <v>23.584</v>
       </c>
       <c r="F35" s="10">
-        <v>47.436999999999998</v>
+        <v>36.384</v>
       </c>
       <c r="G35" s="11">
-        <v>116.6</v>
+        <v>110.1</v>
       </c>
       <c r="H35" s="11">
-        <v>85.5</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
       <c r="J35" s="13">
-        <v>41537</v>
+        <v>42443</v>
       </c>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="C36">
-        <v>2667</v>
+        <v>3066</v>
       </c>
       <c r="D36" s="10">
-        <v>24.206</v>
+        <v>28.776</v>
       </c>
       <c r="E36" s="10">
-        <v>24.602</v>
+        <v>23.881</v>
       </c>
       <c r="F36" s="10">
-        <v>41.085000000000001</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>10</v>
+        <v>47.396000000000001</v>
+      </c>
+      <c r="G36" s="11">
+        <v>103.658</v>
+      </c>
+      <c r="H36" s="11">
+        <v>85.453000000000003</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>64</v>
+        <v>203</v>
       </c>
       <c r="J36" s="13">
-        <v>40683</v>
-      </c>
+        <v>44691</v>
+      </c>
+      <c r="K36" s="5"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="C37">
-        <v>2829</v>
+        <v>3200</v>
       </c>
       <c r="D37" s="10">
-        <v>21.475999999999999</v>
+        <v>37.845999999999997</v>
       </c>
       <c r="E37" s="10">
-        <v>25.608000000000001</v>
+        <v>23.882000000000001</v>
       </c>
       <c r="F37" s="10">
-        <v>30.663</v>
+        <v>47.436999999999998</v>
       </c>
       <c r="G37" s="11">
-        <v>95.2</v>
+        <v>116.6</v>
       </c>
       <c r="H37" s="11">
-        <v>55.3</v>
+        <v>85.5</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="J37" s="13">
-        <v>39896</v>
+        <v>41537</v>
       </c>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C38">
-        <v>3352</v>
+        <v>2667</v>
       </c>
       <c r="D38" s="10">
-        <v>28.021999999999998</v>
+        <v>24.206</v>
       </c>
       <c r="E38" s="10">
-        <v>32.585999999999999</v>
+        <v>24.602</v>
       </c>
       <c r="F38" s="10">
-        <v>44.103999999999999</v>
-      </c>
-      <c r="G38" s="11">
-        <v>122.4</v>
-      </c>
-      <c r="H38" s="11">
-        <v>79.2</v>
+        <v>41.085000000000001</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>67</v>
+        <v>202</v>
       </c>
       <c r="J38" s="13">
-        <v>42315</v>
+        <v>40683</v>
       </c>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C39">
-        <v>3352</v>
+        <v>2829</v>
       </c>
       <c r="D39" s="10">
-        <v>25.033999999999999</v>
+        <v>21.475999999999999</v>
       </c>
       <c r="E39" s="10">
-        <v>32.850999999999999</v>
+        <v>25.608000000000001</v>
       </c>
       <c r="F39" s="10">
-        <v>40.966999999999999</v>
+        <v>30.663</v>
       </c>
       <c r="G39" s="11">
-        <v>117.2</v>
+        <v>95.2</v>
       </c>
       <c r="H39" s="11">
-        <v>73.900000000000006</v>
+        <v>55.3</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>67</v>
+        <v>201</v>
       </c>
       <c r="J39" s="13">
-        <v>42315</v>
+        <v>39896</v>
       </c>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C40">
-        <v>2300</v>
+        <v>2667</v>
       </c>
       <c r="D40" s="10">
-        <v>39.049999999999997</v>
+        <v>27.460999999999999</v>
       </c>
       <c r="E40" s="10">
-        <v>33.215000000000003</v>
+        <v>26.341999999999999</v>
       </c>
       <c r="F40" s="10">
-        <v>54.26</v>
+        <v>27.893999999999998</v>
       </c>
       <c r="G40" s="11">
-        <v>142.69999999999999</v>
+        <v>107.5</v>
       </c>
       <c r="H40" s="11">
-        <v>97.8</v>
+        <v>86.4</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>10</v>
+        <v>211</v>
       </c>
       <c r="J40" s="13">
-        <v>42397</v>
+        <v>43956</v>
       </c>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41">
+        <v>3352</v>
+      </c>
+      <c r="D41" s="10">
+        <v>28.021999999999998</v>
+      </c>
+      <c r="E41" s="10">
+        <v>32.585999999999999</v>
+      </c>
+      <c r="F41" s="10">
+        <v>44.103999999999999</v>
+      </c>
+      <c r="G41" s="11">
+        <v>122.4</v>
+      </c>
+      <c r="H41" s="11">
+        <v>79.2</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="J41" s="13">
+        <v>42315</v>
+      </c>
+      <c r="L41" s="13"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="20">
+        <v>2300</v>
+      </c>
+      <c r="D42" s="10">
+        <v>39.049999999999997</v>
+      </c>
+      <c r="E42" s="10">
+        <v>33.215000000000003</v>
+      </c>
+      <c r="F42" s="10">
+        <v>54.26</v>
+      </c>
+      <c r="G42" s="11">
+        <v>142.69999999999999</v>
+      </c>
+      <c r="H42" s="11">
+        <v>97.8</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" s="13">
+        <v>42397</v>
+      </c>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C41">
+      <c r="C43" s="20">
         <v>2500</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D43" s="10">
         <v>40.698999999999998</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E43" s="10">
         <v>37.018000000000001</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F43" s="10">
         <v>52.634999999999998</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G43" s="11">
         <v>154.5</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H43" s="11">
         <v>94.9</v>
       </c>
-      <c r="I41" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J41" s="13">
+      <c r="I43" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J43" s="13">
         <v>42397</v>
       </c>
-      <c r="L41" s="13"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="L43" s="13"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C42">
+      <c r="C44" s="20">
         <v>2600</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D44" s="10">
         <v>45.381999999999998</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E44" s="10">
         <v>40.313000000000002</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F44" s="10">
         <v>61.804000000000002</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G44" s="11">
         <v>169.9</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H44" s="11">
         <v>111.4</v>
       </c>
-      <c r="I42" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J42" s="13">
+      <c r="I44" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="J44" s="13">
         <v>42817</v>
-      </c>
-      <c r="L42" s="13"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>165</v>
-      </c>
-      <c r="B43" t="s">
-        <v>166</v>
-      </c>
-      <c r="C43">
-        <v>2700</v>
-      </c>
-      <c r="D43" s="10">
-        <v>54.363</v>
-      </c>
-      <c r="E43" s="10">
-        <v>41.972000000000001</v>
-      </c>
-      <c r="F43" s="10">
-        <v>106.893</v>
-      </c>
-      <c r="G43" s="11">
-        <v>187.91900000000001</v>
-      </c>
-      <c r="H43" s="11">
-        <v>192.7</v>
-      </c>
-      <c r="I43" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="J43" s="13">
-        <v>44153</v>
-      </c>
-      <c r="L43" s="13"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>173</v>
-      </c>
-      <c r="B44" t="s">
-        <v>166</v>
-      </c>
-      <c r="C44">
-        <v>2700</v>
-      </c>
-      <c r="D44" s="10">
-        <v>57.2</v>
-      </c>
-      <c r="E44" s="10">
-        <v>43.731999999999999</v>
-      </c>
-      <c r="F44" s="10">
-        <v>107.95399999999999</v>
-      </c>
-      <c r="G44" s="11">
-        <v>196.6</v>
-      </c>
-      <c r="H44" s="11">
-        <v>194.6</v>
-      </c>
-      <c r="J44" s="13">
-        <v>44155</v>
       </c>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>216</v>
+      </c>
+      <c r="B45" t="s">
+        <v>217</v>
+      </c>
+      <c r="C45">
+        <v>2112</v>
+      </c>
+      <c r="D45" s="10">
+        <v>61.249000000000002</v>
+      </c>
+      <c r="E45" s="10">
+        <v>46.226999999999997</v>
+      </c>
+      <c r="F45" s="10">
+        <v>113.619</v>
+      </c>
+      <c r="G45" s="11">
+        <v>209</v>
+      </c>
+      <c r="H45" s="11">
+        <v>204.9</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="J45" s="14">
+        <v>45298</v>
+      </c>
+      <c r="L45" s="13"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C46" s="20">
+        <v>2700</v>
+      </c>
+      <c r="D46" s="10">
+        <v>57.2</v>
+      </c>
+      <c r="E46" s="10">
+        <v>43.731999999999999</v>
+      </c>
+      <c r="F46" s="10">
+        <v>107.95399999999999</v>
+      </c>
+      <c r="G46" s="11">
+        <v>196.6</v>
+      </c>
+      <c r="H46" s="11">
+        <v>194.6</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="J46" s="13">
+        <v>44155</v>
+      </c>
+      <c r="L46" s="13"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C45">
+      <c r="C47" s="20">
         <v>2600</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D47" s="10">
         <v>55.045999999999999</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E47" s="10">
         <v>44.618000000000002</v>
       </c>
-      <c r="F45" s="10">
+      <c r="F47" s="10">
         <v>73.569999999999993</v>
       </c>
-      <c r="G45" s="11">
+      <c r="G47" s="11">
         <v>195.6</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H47" s="11">
         <v>132.6</v>
       </c>
-      <c r="I45" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="J45" s="13">
+      <c r="I47" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="J47" s="13">
         <v>43355</v>
       </c>
-      <c r="K45" s="7"/>
-      <c r="L45" s="13"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="K47" s="7"/>
+      <c r="L47" s="13"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C46">
+      <c r="C48" s="20">
         <v>2600</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D48" s="10">
         <v>63.682000000000002</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E48" s="10">
         <v>45.731999999999999</v>
       </c>
-      <c r="F46" s="10">
+      <c r="F48" s="10">
         <v>68.159000000000006</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G48" s="11">
         <v>211.2</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H48" s="11">
         <v>122.9</v>
       </c>
-      <c r="I46" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J46" s="13">
+      <c r="I48" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J48" s="13">
         <v>43146</v>
       </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="13"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="K48" s="7"/>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="C47">
+      <c r="C49" s="20">
         <v>2500</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D49" s="10">
         <v>50.423000000000002</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E49" s="10">
         <v>46.116999999999997</v>
       </c>
-      <c r="F47" s="10">
+      <c r="F49" s="10">
         <v>70.039000000000001</v>
       </c>
-      <c r="G47" s="11">
+      <c r="G49" s="11">
         <v>192</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H49" s="11">
         <v>126.3</v>
       </c>
-      <c r="I47" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J47" s="13">
+      <c r="I49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" s="13">
         <v>43146</v>
       </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="13"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="K49" s="5"/>
+      <c r="L49" s="13"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>208</v>
+      </c>
+      <c r="B50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C50">
+        <v>3700</v>
+      </c>
+      <c r="D50" s="10">
+        <v>62.206000000000003</v>
+      </c>
+      <c r="E50" s="10">
+        <v>49.951000000000001</v>
+      </c>
+      <c r="F50" s="10">
+        <v>112.593</v>
+      </c>
+      <c r="G50" s="11">
+        <v>219.9</v>
+      </c>
+      <c r="H50" s="11">
+        <v>203</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="J50" s="13">
+        <v>45561</v>
+      </c>
+      <c r="K50" s="5"/>
+      <c r="L50" s="13"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>177</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>178</v>
       </c>
-      <c r="C48">
-        <v>3600</v>
-      </c>
-      <c r="D48" s="10">
+      <c r="C51">
+        <v>4160</v>
+      </c>
+      <c r="D51" s="10">
         <v>77.174000000000007</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E51" s="10">
         <v>56.761000000000003</v>
       </c>
-      <c r="F48" s="10">
+      <c r="F51" s="10">
         <v>138.00299999999999</v>
       </c>
-      <c r="G48" s="11">
+      <c r="G51" s="11">
         <v>259.47000000000003</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H51" s="11">
         <v>248.81200000000001</v>
       </c>
-      <c r="I48" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="J48" s="14">
+      <c r="I51" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="J51" s="14">
         <v>45211</v>
       </c>
-      <c r="K48" s="5"/>
-      <c r="L48" s="13"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>167</v>
-      </c>
-      <c r="B49" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49">
-        <v>2667</v>
-      </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J49" s="13">
-        <v>43956</v>
-      </c>
-      <c r="L49" s="13"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F50" s="10"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="J50" s="7"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F51" s="10"/>
-      <c r="J51" s="7"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="13"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J52" s="7"/>
+      <c r="A52" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C52" s="20">
+        <v>3200</v>
+      </c>
+      <c r="D52" s="22">
+        <v>66.938999999999993</v>
+      </c>
+      <c r="E52" s="22">
+        <v>79.733000000000004</v>
+      </c>
+      <c r="F52" s="22">
+        <v>216.304</v>
+      </c>
+      <c r="G52" s="23">
+        <v>296.39999999999998</v>
+      </c>
+      <c r="H52" s="23">
+        <v>389.9</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" s="24">
+        <v>45561</v>
+      </c>
+      <c r="K52" s="5"/>
+      <c r="L52" s="13"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J53" s="7"/>
+      <c r="A53" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53">
+        <v>4700</v>
+      </c>
+      <c r="D53" s="10">
+        <v>104.52500000000001</v>
+      </c>
+      <c r="E53" s="10">
+        <v>85.01</v>
+      </c>
+      <c r="F53" s="10">
+        <v>264.86900000000003</v>
+      </c>
+      <c r="G53" s="11">
+        <v>372.2</v>
+      </c>
+      <c r="H53" s="11">
+        <v>377.5</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="J53" s="14">
+        <v>45561</v>
+      </c>
+      <c r="K53" s="5"/>
+      <c r="L53" s="13"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J54" s="7"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="13"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F55" s="10"/>
+      <c r="J55" s="7"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J56" s="7"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J57" s="7"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J58" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J49">
-    <sortCondition ref="E2:E49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J53">
+    <sortCondition ref="E2:E53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8361,6 +8649,22 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
@@ -8369,22 +8673,6 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="http://pdadb.net/index.php?m=cpu&amp;id=a6422&amp;c=samsung_s5p6422" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>